<commit_message>
Finalizado con todo de Programacion Estructurada
</commit_message>
<xml_diff>
--- a/OYM/_Documentos Comunes/PE_C32017.xlsx
+++ b/OYM/_Documentos Comunes/PE_C32017.xlsx
@@ -1521,9 +1521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W33" sqref="W33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2247,9 +2247,12 @@
       <c r="W20">
         <v>18</v>
       </c>
+      <c r="X20">
+        <v>30</v>
+      </c>
       <c r="Y20">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="Z20">
         <v>5</v>
@@ -2292,9 +2295,12 @@
       <c r="W21">
         <v>16</v>
       </c>
+      <c r="X21">
+        <v>30</v>
+      </c>
       <c r="Y21">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="Z21">
         <v>5</v>
@@ -2425,11 +2431,11 @@
         <v>17</v>
       </c>
       <c r="X24">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="Y24">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="Z24">
         <v>5</v>
@@ -2646,9 +2652,12 @@
       <c r="W30">
         <v>16</v>
       </c>
+      <c r="X30">
+        <v>30</v>
+      </c>
       <c r="Y30">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="Z30">
         <v>5</v>
@@ -2685,9 +2694,12 @@
       <c r="W31">
         <v>18</v>
       </c>
+      <c r="X31">
+        <v>30</v>
+      </c>
       <c r="Y31">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="Z31">
         <v>5</v>
@@ -2727,9 +2739,12 @@
       <c r="W32">
         <v>18</v>
       </c>
+      <c r="X32">
+        <v>30</v>
+      </c>
       <c r="Y32">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="Z32">
         <v>5</v>
@@ -2769,9 +2784,12 @@
       <c r="W33">
         <v>19</v>
       </c>
+      <c r="X33">
+        <v>30</v>
+      </c>
       <c r="Y33">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="Z33">
         <v>5</v>
@@ -2979,9 +2997,12 @@
       <c r="W38">
         <v>18</v>
       </c>
+      <c r="X38">
+        <v>30</v>
+      </c>
       <c r="Y38">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="Z38">
         <v>5</v>
@@ -3165,9 +3186,12 @@
       <c r="W42">
         <v>18</v>
       </c>
+      <c r="X42">
+        <v>30</v>
+      </c>
       <c r="Y42">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="Z42">
         <v>5</v>
@@ -3396,9 +3420,12 @@
       <c r="W47">
         <v>16</v>
       </c>
+      <c r="X47">
+        <v>30</v>
+      </c>
       <c r="Y47">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="Z47">
         <v>5</v>
@@ -3507,9 +3534,12 @@
       <c r="W50">
         <v>14</v>
       </c>
+      <c r="X50">
+        <v>30</v>
+      </c>
       <c r="Y50">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="Z50">
         <v>5</v>
@@ -3630,9 +3660,12 @@
       <c r="W53">
         <v>17</v>
       </c>
+      <c r="X53">
+        <v>30</v>
+      </c>
       <c r="Y53">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="Z53">
         <v>5</v>
@@ -3816,9 +3849,12 @@
       <c r="W57">
         <v>18</v>
       </c>
+      <c r="X57">
+        <v>30</v>
+      </c>
       <c r="Y57">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="Z57">
         <v>5</v>
@@ -3903,9 +3939,12 @@
       <c r="W59">
         <v>12</v>
       </c>
+      <c r="X59">
+        <v>30</v>
+      </c>
       <c r="Y59">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="Z59">
         <v>5</v>
@@ -3988,7 +4027,7 @@
         <v>5</v>
       </c>
       <c r="U61">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="V61">
         <v>2</v>
@@ -3996,9 +4035,12 @@
       <c r="W61">
         <v>16</v>
       </c>
+      <c r="X61">
+        <v>30</v>
+      </c>
       <c r="Y61">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="Z61">
         <v>5</v>
@@ -4041,9 +4083,12 @@
       <c r="W62">
         <v>18</v>
       </c>
+      <c r="X62">
+        <v>30</v>
+      </c>
       <c r="Y62">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="Z62">
         <v>5</v>
@@ -4317,9 +4362,12 @@
       <c r="W68">
         <v>15</v>
       </c>
+      <c r="X68">
+        <v>30</v>
+      </c>
       <c r="Y68">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="Z68">
         <v>5</v>
@@ -4410,9 +4458,12 @@
       <c r="W70">
         <v>18</v>
       </c>
+      <c r="X70">
+        <v>30</v>
+      </c>
       <c r="Y70">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="Z70">
         <v>5</v>
@@ -4455,9 +4506,12 @@
       <c r="W71">
         <v>12</v>
       </c>
+      <c r="X71">
+        <v>30</v>
+      </c>
       <c r="Y71">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="Z71">
         <v>5</v>
@@ -5067,9 +5121,12 @@
       <c r="W84">
         <v>12</v>
       </c>
+      <c r="X84">
+        <v>30</v>
+      </c>
       <c r="Y84">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="Z84">
         <v>5</v>
@@ -5284,11 +5341,11 @@
         <v>19</v>
       </c>
       <c r="X89">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="Y89">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="Z89">
         <v>5</v>
@@ -5331,9 +5388,12 @@
       <c r="W90">
         <v>18</v>
       </c>
+      <c r="X90">
+        <v>30</v>
+      </c>
       <c r="Y90">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="Z90">
         <v>5</v>
@@ -5370,9 +5430,12 @@
       <c r="W91">
         <v>15</v>
       </c>
+      <c r="X91">
+        <v>30</v>
+      </c>
       <c r="Y91">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="Z91">
         <v>5</v>

</xml_diff>

<commit_message>
Ya estan todas corregidas, felicidades a los que pasaron, buena suerte en la proxima al resto
</commit_message>
<xml_diff>
--- a/OYM/_Documentos Comunes/PE_C32017.xlsx
+++ b/OYM/_Documentos Comunes/PE_C32017.xlsx
@@ -1521,9 +1521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z108" sqref="Z108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1543,7 +1543,9 @@
     <col min="14" max="15" width="0.140625" customWidth="1"/>
     <col min="16" max="16" width="4.7109375" customWidth="1"/>
     <col min="17" max="17" width="4.5703125" customWidth="1"/>
-    <col min="18" max="20" width="2.5703125" customWidth="1"/>
+    <col min="18" max="18" width="3.42578125" customWidth="1"/>
+    <col min="19" max="19" width="3" customWidth="1"/>
+    <col min="20" max="20" width="3.28515625" customWidth="1"/>
     <col min="21" max="21" width="6.85546875" customWidth="1"/>
     <col min="22" max="22" width="3.7109375" customWidth="1"/>
     <col min="23" max="23" width="8" bestFit="1" customWidth="1"/>
@@ -1817,17 +1819,20 @@
       <c r="F11" s="13"/>
       <c r="G11" s="12"/>
       <c r="H11" s="14">
+        <f>IF((Y11)&gt;70,10,"")</f>
         <v>10</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="5">
+        <f>IF((Y11)&gt;70,20,"")</f>
         <v>20</v>
       </c>
       <c r="K11" s="5">
+        <f>IF((Y11)&gt;70,20,"")</f>
         <v>20</v>
       </c>
       <c r="L11" s="14">
-        <f>IF((Y11-50)&gt;50,50,IF((Y11-50)&lt;0,0,(Y11-50)))</f>
+        <f>IF((Y11)&gt;70,IF((Y11-50)&gt;50,50,IF((Y11-50)&lt;0,0,(Y11-50))), "" )</f>
         <v>50</v>
       </c>
       <c r="M11" s="22"/>
@@ -1882,11 +1887,23 @@
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="14"/>
+      <c r="H12" s="14">
+        <f t="shared" ref="H12:H75" si="0">IF((Y12)&gt;70,10,"")</f>
+        <v>10</v>
+      </c>
       <c r="I12" s="15"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="14"/>
+      <c r="J12" s="5">
+        <f t="shared" ref="J12:J75" si="1">IF((Y12)&gt;70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" ref="K12:K75" si="2">IF((Y12)&gt;70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="L12" s="14">
+        <f t="shared" ref="L12:L75" si="3">IF((Y12)&gt;70,IF((Y12-50)&gt;50,50,IF((Y12-50)&lt;0,0,(Y12-50))), "" )</f>
+        <v>41</v>
+      </c>
       <c r="M12" s="22"/>
       <c r="N12" s="15"/>
       <c r="O12" s="2"/>
@@ -1903,7 +1920,7 @@
         <v>18</v>
       </c>
       <c r="Y12">
-        <f t="shared" ref="Y12:Y75" si="0">P12+(IF((Q12+R12+S12+T12)&gt;30,(Q12+R12+S12+T12)/4,IF((Q12+R12+S12+T12)&gt;20,(Q12+R12+S12+T12)/3,IF((Q12+R12+S12+T12)&gt;10,(Q12+R12+S12+T12)/2,(Q12+R12+S12+T12)))))+(U12*V12)+W12+X12+Z12</f>
+        <f t="shared" ref="Y12:Y75" si="4">P12+(IF((Q12+R12+S12+T12)&gt;30,(Q12+R12+S12+T12)/4,IF((Q12+R12+S12+T12)&gt;20,(Q12+R12+S12+T12)/3,IF((Q12+R12+S12+T12)&gt;10,(Q12+R12+S12+T12)/2,(Q12+R12+S12+T12)))))+(U12*V12)+W12+X12+Z12</f>
         <v>91</v>
       </c>
       <c r="Z12">
@@ -1924,11 +1941,23 @@
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="14"/>
+      <c r="H13" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I13" s="15"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="14"/>
+      <c r="J13" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L13" s="14">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
       <c r="M13" s="22"/>
       <c r="N13" s="15"/>
       <c r="O13" s="2"/>
@@ -1951,7 +1980,7 @@
         <v>10</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="Z13">
@@ -1972,11 +2001,23 @@
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="20"/>
-      <c r="H14" s="14"/>
+      <c r="H14" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I14" s="15"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="14"/>
+      <c r="J14" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L14" s="14">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
       <c r="M14" s="22"/>
       <c r="N14" s="15"/>
       <c r="O14" s="2"/>
@@ -1999,7 +2040,7 @@
         <v>30</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="Z14">
@@ -2020,11 +2061,23 @@
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="20"/>
-      <c r="H15" s="14"/>
+      <c r="H15" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I15" s="15"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="14"/>
+      <c r="J15" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L15" s="14">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
       <c r="M15" s="22"/>
       <c r="N15" s="15"/>
       <c r="O15" s="2"/>
@@ -2044,7 +2097,7 @@
         <v>30</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
       <c r="Z15">
@@ -2065,11 +2118,23 @@
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="20"/>
-      <c r="H16" s="14"/>
+      <c r="H16" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I16" s="15"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="14"/>
+      <c r="J16" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
       <c r="M16" s="22"/>
       <c r="N16" s="15"/>
       <c r="O16" s="2"/>
@@ -2089,7 +2154,7 @@
         <v>17</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
       <c r="Z16">
@@ -2110,11 +2175,23 @@
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="20"/>
-      <c r="H17" s="14"/>
+      <c r="H17" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I17" s="15"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="14"/>
+      <c r="J17" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K17" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L17" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M17" s="22"/>
       <c r="N17" s="15"/>
       <c r="O17" s="2"/>
@@ -2122,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="Z17">
@@ -2143,11 +2220,23 @@
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="20"/>
-      <c r="H18" s="14"/>
+      <c r="H18" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I18" s="15"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="14"/>
+      <c r="J18" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L18" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M18" s="22"/>
       <c r="N18" s="15"/>
       <c r="O18" s="2"/>
@@ -2170,7 +2259,7 @@
         <v>30</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>112</v>
       </c>
       <c r="Z18">
@@ -2191,11 +2280,23 @@
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="20"/>
-      <c r="H19" s="14"/>
+      <c r="H19" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I19" s="15"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="14"/>
+      <c r="J19" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K19" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L19" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M19" s="22"/>
       <c r="N19" s="15"/>
       <c r="O19" s="2"/>
@@ -2206,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="Z19">
@@ -2227,11 +2328,23 @@
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="20"/>
-      <c r="H20" s="14"/>
+      <c r="H20" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I20" s="15"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="14"/>
+      <c r="J20" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L20" s="14">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
       <c r="M20" s="22"/>
       <c r="N20" s="15"/>
       <c r="O20" s="2"/>
@@ -2251,7 +2364,7 @@
         <v>30</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="Z20">
@@ -2272,11 +2385,23 @@
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="20"/>
-      <c r="H21" s="14"/>
+      <c r="H21" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I21" s="15"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="14"/>
+      <c r="J21" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L21" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M21" s="22"/>
       <c r="N21" s="15"/>
       <c r="O21" s="2"/>
@@ -2299,7 +2424,7 @@
         <v>30</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="Z21">
@@ -2320,11 +2445,23 @@
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="20"/>
-      <c r="H22" s="14"/>
+      <c r="H22" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I22" s="15"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="14"/>
+      <c r="J22" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L22" s="14">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
       <c r="M22" s="22"/>
       <c r="N22" s="15"/>
       <c r="O22" s="2"/>
@@ -2344,7 +2481,7 @@
         <v>30</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="Z22">
@@ -2365,11 +2502,23 @@
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="20"/>
-      <c r="H23" s="14"/>
+      <c r="H23" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I23" s="15"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="14"/>
+      <c r="J23" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K23" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L23" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M23" s="22"/>
       <c r="N23" s="15"/>
       <c r="O23" s="2"/>
@@ -2386,7 +2535,7 @@
         <v>20</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="Z23">
@@ -2407,11 +2556,23 @@
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="20"/>
-      <c r="H24" s="14"/>
+      <c r="H24" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="14"/>
+      <c r="J24" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L24" s="14">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
       <c r="M24" s="22"/>
       <c r="N24" s="15"/>
       <c r="O24" s="2"/>
@@ -2434,7 +2595,7 @@
         <v>-1</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="Z24">
@@ -2455,11 +2616,23 @@
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="20"/>
-      <c r="H25" s="14"/>
+      <c r="H25" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I25" s="15"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="14"/>
+      <c r="J25" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K25" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L25" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M25" s="22"/>
       <c r="N25" s="15"/>
       <c r="O25" s="2"/>
@@ -2467,7 +2640,7 @@
         <v>1</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="Z25">
@@ -2488,11 +2661,23 @@
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="20"/>
-      <c r="H26" s="14"/>
+      <c r="H26" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I26" s="15"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="14"/>
+      <c r="J26" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K26" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L26" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M26" s="22"/>
       <c r="N26" s="15"/>
       <c r="O26" s="2"/>
@@ -2500,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="Z26">
@@ -2521,11 +2706,23 @@
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="20"/>
-      <c r="H27" s="14"/>
+      <c r="H27" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I27" s="15"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="14"/>
+      <c r="J27" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K27" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L27" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M27" s="22"/>
       <c r="N27" s="15"/>
       <c r="O27" s="2"/>
@@ -2542,11 +2739,11 @@
         <v>30</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="0"/>
-        <v>63</v>
+        <f t="shared" si="4"/>
+        <v>70</v>
       </c>
       <c r="Z27">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2563,11 +2760,23 @@
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="20"/>
-      <c r="H28" s="14"/>
+      <c r="H28" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I28" s="15"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="14"/>
+      <c r="J28" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K28" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L28" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M28" s="22"/>
       <c r="N28" s="15"/>
       <c r="O28" s="2"/>
@@ -2578,7 +2787,7 @@
         <v>1</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="Z28">
@@ -2599,11 +2808,23 @@
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="20"/>
-      <c r="H29" s="14"/>
+      <c r="H29" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I29" s="15"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="14"/>
+      <c r="J29" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K29" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L29" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M29" s="22"/>
       <c r="N29" s="15"/>
       <c r="O29" s="2"/>
@@ -2611,7 +2832,7 @@
         <v>1</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="Z29">
@@ -2632,11 +2853,23 @@
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="20"/>
-      <c r="H30" s="14"/>
+      <c r="H30" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I30" s="15"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="14"/>
+      <c r="J30" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L30" s="14">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
       <c r="M30" s="22"/>
       <c r="N30" s="15"/>
       <c r="O30" s="2"/>
@@ -2656,7 +2889,7 @@
         <v>30</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
       <c r="Z30">
@@ -2677,11 +2910,23 @@
       </c>
       <c r="F31" s="21"/>
       <c r="G31" s="20"/>
-      <c r="H31" s="14"/>
+      <c r="H31" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I31" s="15"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="14"/>
+      <c r="J31" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L31" s="14">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
       <c r="M31" s="22"/>
       <c r="N31" s="15"/>
       <c r="O31" s="2"/>
@@ -2698,7 +2943,7 @@
         <v>30</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>87</v>
       </c>
       <c r="Z31">
@@ -2719,11 +2964,23 @@
       </c>
       <c r="F32" s="21"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="14"/>
+      <c r="H32" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I32" s="15"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="14"/>
+      <c r="J32" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L32" s="14">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
       <c r="M32" s="22"/>
       <c r="N32" s="15"/>
       <c r="O32" s="2"/>
@@ -2743,7 +3000,7 @@
         <v>30</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="Z32">
@@ -2764,11 +3021,23 @@
       </c>
       <c r="F33" s="21"/>
       <c r="G33" s="20"/>
-      <c r="H33" s="14"/>
+      <c r="H33" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I33" s="15"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="14"/>
+      <c r="J33" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L33" s="14">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
       <c r="M33" s="22"/>
       <c r="N33" s="15"/>
       <c r="O33" s="2"/>
@@ -2788,7 +3057,7 @@
         <v>30</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="Z33">
@@ -2809,11 +3078,23 @@
       </c>
       <c r="F34" s="21"/>
       <c r="G34" s="20"/>
-      <c r="H34" s="14"/>
+      <c r="H34" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I34" s="15"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="14"/>
+      <c r="J34" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K34" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L34" s="14">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
       <c r="M34" s="22"/>
       <c r="N34" s="15"/>
       <c r="O34" s="2"/>
@@ -2821,14 +3102,14 @@
         <v>16</v>
       </c>
       <c r="V34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W34">
         <v>18</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <f t="shared" si="4"/>
+        <v>75</v>
       </c>
       <c r="Z34">
         <v>25</v>
@@ -2848,11 +3129,23 @@
       </c>
       <c r="F35" s="21"/>
       <c r="G35" s="20"/>
-      <c r="H35" s="14"/>
+      <c r="H35" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I35" s="15"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="14"/>
+      <c r="J35" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L35" s="14">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
       <c r="M35" s="22"/>
       <c r="N35" s="15"/>
       <c r="O35" s="2"/>
@@ -2869,7 +3162,7 @@
         <v>30</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
       <c r="Z35">
@@ -2890,11 +3183,23 @@
       </c>
       <c r="F36" s="21"/>
       <c r="G36" s="20"/>
-      <c r="H36" s="14"/>
+      <c r="H36" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I36" s="15"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="14"/>
+      <c r="J36" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L36" s="14">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
       <c r="M36" s="22"/>
       <c r="N36" s="15"/>
       <c r="O36" s="2"/>
@@ -2914,7 +3219,7 @@
         <v>30</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="Z36">
@@ -2935,11 +3240,23 @@
       </c>
       <c r="F37" s="21"/>
       <c r="G37" s="20"/>
-      <c r="H37" s="14"/>
+      <c r="H37" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I37" s="15"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="14"/>
+      <c r="J37" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K37" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L37" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M37" s="22"/>
       <c r="N37" s="15"/>
       <c r="O37" s="2"/>
@@ -2956,11 +3273,11 @@
         <v>18</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="0"/>
-        <v>68</v>
+        <f t="shared" si="4"/>
+        <v>70</v>
       </c>
       <c r="Z37">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2977,11 +3294,23 @@
       </c>
       <c r="F38" s="21"/>
       <c r="G38" s="20"/>
-      <c r="H38" s="14"/>
+      <c r="H38" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I38" s="15"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="14"/>
+      <c r="J38" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K38" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L38" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M38" s="22"/>
       <c r="N38" s="15"/>
       <c r="O38" s="2"/>
@@ -3001,7 +3330,7 @@
         <v>30</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>102</v>
       </c>
       <c r="Z38">
@@ -3022,11 +3351,23 @@
       </c>
       <c r="F39" s="21"/>
       <c r="G39" s="20"/>
-      <c r="H39" s="14"/>
+      <c r="H39" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I39" s="15"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="14"/>
+      <c r="J39" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L39" s="14">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
       <c r="M39" s="22"/>
       <c r="N39" s="15"/>
       <c r="O39" s="2"/>
@@ -3049,7 +3390,7 @@
         <v>20</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
       <c r="Z39">
@@ -3070,11 +3411,23 @@
       </c>
       <c r="F40" s="21"/>
       <c r="G40" s="20"/>
-      <c r="H40" s="14"/>
+      <c r="H40" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I40" s="15"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="14"/>
+      <c r="J40" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K40" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L40" s="14">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
       <c r="M40" s="22"/>
       <c r="N40" s="15"/>
       <c r="O40" s="2"/>
@@ -3094,7 +3447,7 @@
         <v>20</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>87</v>
       </c>
       <c r="Z40">
@@ -3115,11 +3468,23 @@
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="20"/>
-      <c r="H41" s="14"/>
+      <c r="H41" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I41" s="15"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="14"/>
+      <c r="J41" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L41" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M41" s="22"/>
       <c r="N41" s="15"/>
       <c r="O41" s="2"/>
@@ -3142,7 +3507,7 @@
         <v>30</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
       <c r="Z41">
@@ -3163,11 +3528,23 @@
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="20"/>
-      <c r="H42" s="14"/>
+      <c r="H42" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I42" s="15"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="14"/>
+      <c r="J42" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L42" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M42" s="22"/>
       <c r="N42" s="15"/>
       <c r="O42" s="2"/>
@@ -3190,7 +3567,7 @@
         <v>30</v>
       </c>
       <c r="Y42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>111</v>
       </c>
       <c r="Z42">
@@ -3211,11 +3588,23 @@
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="20"/>
-      <c r="H43" s="14"/>
+      <c r="H43" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I43" s="15"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="14"/>
+      <c r="J43" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L43" s="14">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
       <c r="M43" s="22"/>
       <c r="N43" s="15"/>
       <c r="O43" s="2"/>
@@ -3238,7 +3627,7 @@
         <v>20</v>
       </c>
       <c r="Y43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="Z43">
@@ -3259,11 +3648,23 @@
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="20"/>
-      <c r="H44" s="14"/>
+      <c r="H44" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I44" s="15"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="14"/>
+      <c r="J44" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L44" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M44" s="22"/>
       <c r="N44" s="15"/>
       <c r="O44" s="2"/>
@@ -3286,7 +3687,7 @@
         <v>30</v>
       </c>
       <c r="Y44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>103</v>
       </c>
       <c r="Z44">
@@ -3307,11 +3708,23 @@
       </c>
       <c r="F45" s="21"/>
       <c r="G45" s="20"/>
-      <c r="H45" s="14"/>
+      <c r="H45" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I45" s="15"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="14"/>
+      <c r="J45" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L45" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M45" s="22"/>
       <c r="N45" s="15"/>
       <c r="O45" s="2"/>
@@ -3334,7 +3747,7 @@
         <v>30</v>
       </c>
       <c r="Y45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>105</v>
       </c>
       <c r="Z45">
@@ -3355,11 +3768,23 @@
       </c>
       <c r="F46" s="21"/>
       <c r="G46" s="20"/>
-      <c r="H46" s="14"/>
+      <c r="H46" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I46" s="15"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="14"/>
+      <c r="J46" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K46" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L46" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M46" s="22"/>
       <c r="N46" s="15"/>
       <c r="O46" s="2"/>
@@ -3379,7 +3804,7 @@
         <v>30</v>
       </c>
       <c r="Y46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
       <c r="Z46">
@@ -3400,11 +3825,23 @@
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="20"/>
-      <c r="H47" s="14"/>
+      <c r="H47" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I47" s="15"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="14"/>
+      <c r="J47" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K47" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L47" s="14">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
       <c r="M47" s="22"/>
       <c r="N47" s="15"/>
       <c r="O47" s="2"/>
@@ -3424,7 +3861,7 @@
         <v>30</v>
       </c>
       <c r="Y47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="Z47">
@@ -3445,11 +3882,23 @@
       </c>
       <c r="F48" s="21"/>
       <c r="G48" s="20"/>
-      <c r="H48" s="14"/>
+      <c r="H48" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I48" s="15"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="14"/>
+      <c r="J48" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K48" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L48" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M48" s="22"/>
       <c r="N48" s="15"/>
       <c r="O48" s="2"/>
@@ -3457,7 +3906,7 @@
         <v>1</v>
       </c>
       <c r="Y48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="Z48">
@@ -3478,11 +3927,23 @@
       </c>
       <c r="F49" s="21"/>
       <c r="G49" s="20"/>
-      <c r="H49" s="14"/>
+      <c r="H49" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I49" s="15"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="14"/>
+      <c r="J49" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K49" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L49" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M49" s="22"/>
       <c r="N49" s="15"/>
       <c r="O49" s="2"/>
@@ -3493,7 +3954,7 @@
         <v>1</v>
       </c>
       <c r="Y49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="Z49">
@@ -3514,11 +3975,23 @@
       </c>
       <c r="F50" s="21"/>
       <c r="G50" s="20"/>
-      <c r="H50" s="14"/>
+      <c r="H50" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I50" s="15"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="14"/>
+      <c r="J50" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K50" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L50" s="14">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
       <c r="M50" s="22"/>
       <c r="N50" s="15"/>
       <c r="O50" s="2"/>
@@ -3538,7 +4011,7 @@
         <v>30</v>
       </c>
       <c r="Y50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
       <c r="Z50">
@@ -3559,11 +4032,23 @@
       </c>
       <c r="F51" s="21"/>
       <c r="G51" s="20"/>
-      <c r="H51" s="14"/>
+      <c r="H51" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I51" s="15"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="14"/>
+      <c r="J51" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K51" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L51" s="14">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
       <c r="M51" s="22"/>
       <c r="N51" s="15"/>
       <c r="O51" s="2"/>
@@ -3580,7 +4065,7 @@
         <v>17</v>
       </c>
       <c r="Y51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
       <c r="Z51">
@@ -3601,11 +4086,23 @@
       </c>
       <c r="F52" s="21"/>
       <c r="G52" s="20"/>
-      <c r="H52" s="14"/>
+      <c r="H52" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I52" s="15"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="14"/>
+      <c r="J52" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K52" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L52" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M52" s="22"/>
       <c r="N52" s="15"/>
       <c r="O52" s="2"/>
@@ -3616,7 +4113,7 @@
         <v>1</v>
       </c>
       <c r="Y52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="Z52">
@@ -3637,11 +4134,23 @@
       </c>
       <c r="F53" s="21"/>
       <c r="G53" s="20"/>
-      <c r="H53" s="14"/>
+      <c r="H53" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I53" s="15"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="14"/>
+      <c r="J53" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K53" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L53" s="14">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
       <c r="M53" s="22"/>
       <c r="N53" s="15"/>
       <c r="O53" s="2"/>
@@ -3664,7 +4173,7 @@
         <v>30</v>
       </c>
       <c r="Y53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="Z53">
@@ -3685,11 +4194,23 @@
       </c>
       <c r="F54" s="21"/>
       <c r="G54" s="20"/>
-      <c r="H54" s="14"/>
+      <c r="H54" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I54" s="15"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="14"/>
+      <c r="J54" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K54" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L54" s="14">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
       <c r="M54" s="22"/>
       <c r="N54" s="15"/>
       <c r="O54" s="2"/>
@@ -3712,7 +4233,7 @@
         <v>30</v>
       </c>
       <c r="Y54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="Z54">
@@ -3733,11 +4254,23 @@
       </c>
       <c r="F55" s="21"/>
       <c r="G55" s="20"/>
-      <c r="H55" s="14"/>
+      <c r="H55" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I55" s="15"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="14"/>
+      <c r="J55" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K55" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L55" s="14">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
       <c r="M55" s="22"/>
       <c r="N55" s="15"/>
       <c r="O55" s="2"/>
@@ -3757,7 +4290,7 @@
         <v>30</v>
       </c>
       <c r="Y55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="Z55">
@@ -3778,11 +4311,23 @@
       </c>
       <c r="F56" s="21"/>
       <c r="G56" s="20"/>
-      <c r="H56" s="14"/>
+      <c r="H56" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I56" s="15"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="14"/>
+      <c r="J56" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K56" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L56" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M56" s="22"/>
       <c r="N56" s="15"/>
       <c r="O56" s="2"/>
@@ -3805,7 +4350,7 @@
         <v>30</v>
       </c>
       <c r="Y56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>103</v>
       </c>
       <c r="Z56">
@@ -3826,11 +4371,23 @@
       </c>
       <c r="F57" s="21"/>
       <c r="G57" s="20"/>
-      <c r="H57" s="14"/>
+      <c r="H57" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I57" s="15"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="14"/>
+      <c r="J57" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K57" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L57" s="14">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
       <c r="M57" s="22"/>
       <c r="N57" s="15"/>
       <c r="O57" s="2"/>
@@ -3853,7 +4410,7 @@
         <v>30</v>
       </c>
       <c r="Y57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
       <c r="Z57">
@@ -3874,11 +4431,23 @@
       </c>
       <c r="F58" s="21"/>
       <c r="G58" s="20"/>
-      <c r="H58" s="14"/>
+      <c r="H58" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I58" s="15"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="14"/>
+      <c r="J58" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K58" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L58" s="14">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
       <c r="M58" s="22"/>
       <c r="N58" s="15"/>
       <c r="O58" s="2"/>
@@ -3895,7 +4464,7 @@
         <v>16</v>
       </c>
       <c r="Y58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="Z58">
@@ -3916,11 +4485,23 @@
       </c>
       <c r="F59" s="21"/>
       <c r="G59" s="20"/>
-      <c r="H59" s="14"/>
+      <c r="H59" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I59" s="15"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="14"/>
+      <c r="J59" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K59" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L59" s="14">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
       <c r="M59" s="22"/>
       <c r="N59" s="15"/>
       <c r="O59" s="2"/>
@@ -3943,7 +4524,7 @@
         <v>30</v>
       </c>
       <c r="Y59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="Z59">
@@ -3964,11 +4545,23 @@
       </c>
       <c r="F60" s="21"/>
       <c r="G60" s="20"/>
-      <c r="H60" s="14"/>
+      <c r="H60" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I60" s="15"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="14"/>
+      <c r="J60" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K60" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L60" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M60" s="22"/>
       <c r="N60" s="15"/>
       <c r="O60" s="2"/>
@@ -3991,7 +4584,7 @@
         <v>30</v>
       </c>
       <c r="Y60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>117</v>
       </c>
       <c r="Z60">
@@ -4012,11 +4605,23 @@
       </c>
       <c r="F61" s="21"/>
       <c r="G61" s="20"/>
-      <c r="H61" s="14"/>
+      <c r="H61" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I61" s="15"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="14"/>
+      <c r="J61" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K61" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L61" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M61" s="22"/>
       <c r="N61" s="15"/>
       <c r="O61" s="2"/>
@@ -4039,7 +4644,7 @@
         <v>30</v>
       </c>
       <c r="Y61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>117</v>
       </c>
       <c r="Z61">
@@ -4060,11 +4665,23 @@
       </c>
       <c r="F62" s="21"/>
       <c r="G62" s="20"/>
-      <c r="H62" s="14"/>
+      <c r="H62" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I62" s="15"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="14"/>
+      <c r="J62" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K62" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L62" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M62" s="22"/>
       <c r="N62" s="15"/>
       <c r="O62" s="2"/>
@@ -4087,7 +4704,7 @@
         <v>30</v>
       </c>
       <c r="Y62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>111</v>
       </c>
       <c r="Z62">
@@ -4108,11 +4725,23 @@
       </c>
       <c r="F63" s="21"/>
       <c r="G63" s="20"/>
-      <c r="H63" s="14"/>
+      <c r="H63" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I63" s="15"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="14"/>
+      <c r="J63" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K63" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L63" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M63" s="22"/>
       <c r="N63" s="15"/>
       <c r="O63" s="2"/>
@@ -4135,7 +4764,7 @@
         <v>30</v>
       </c>
       <c r="Y63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>109</v>
       </c>
       <c r="Z63">
@@ -4156,11 +4785,23 @@
       </c>
       <c r="F64" s="21"/>
       <c r="G64" s="20"/>
-      <c r="H64" s="14"/>
+      <c r="H64" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I64" s="15"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="14"/>
+      <c r="J64" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K64" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L64" s="14">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
       <c r="M64" s="22"/>
       <c r="N64" s="15"/>
       <c r="O64" s="2"/>
@@ -4183,7 +4824,7 @@
         <v>30</v>
       </c>
       <c r="Y64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
       <c r="Z64">
@@ -4204,11 +4845,23 @@
       </c>
       <c r="F65" s="21"/>
       <c r="G65" s="20"/>
-      <c r="H65" s="14"/>
+      <c r="H65" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I65" s="15"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="14"/>
+      <c r="J65" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K65" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L65" s="14">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
       <c r="M65" s="22"/>
       <c r="N65" s="15"/>
       <c r="O65" s="2"/>
@@ -4228,7 +4881,7 @@
         <v>18</v>
       </c>
       <c r="Y65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="Z65">
@@ -4249,11 +4902,23 @@
       </c>
       <c r="F66" s="21"/>
       <c r="G66" s="20"/>
-      <c r="H66" s="14"/>
+      <c r="H66" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="I66" s="15"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="14"/>
+      <c r="J66" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K66" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="L66" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="M66" s="22"/>
       <c r="N66" s="15"/>
       <c r="O66" s="2"/>
@@ -4270,7 +4935,7 @@
         <v>14</v>
       </c>
       <c r="Y66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="Z66">
@@ -4291,11 +4956,23 @@
       </c>
       <c r="F67" s="21"/>
       <c r="G67" s="20"/>
-      <c r="H67" s="14"/>
+      <c r="H67" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I67" s="15"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="14"/>
+      <c r="J67" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K67" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L67" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M67" s="22"/>
       <c r="N67" s="15"/>
       <c r="O67" s="2"/>
@@ -4318,7 +4995,7 @@
         <v>30</v>
       </c>
       <c r="Y67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
       <c r="Z67">
@@ -4339,11 +5016,23 @@
       </c>
       <c r="F68" s="21"/>
       <c r="G68" s="20"/>
-      <c r="H68" s="14"/>
+      <c r="H68" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I68" s="15"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="14"/>
+      <c r="J68" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K68" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L68" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M68" s="22"/>
       <c r="N68" s="15"/>
       <c r="O68" s="2"/>
@@ -4366,7 +5055,7 @@
         <v>30</v>
       </c>
       <c r="Y68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="Z68">
@@ -4387,11 +5076,23 @@
       </c>
       <c r="F69" s="21"/>
       <c r="G69" s="20"/>
-      <c r="H69" s="14"/>
+      <c r="H69" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I69" s="15"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="14"/>
+      <c r="J69" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K69" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L69" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M69" s="22"/>
       <c r="N69" s="15"/>
       <c r="O69" s="2"/>
@@ -4414,7 +5115,7 @@
         <v>30</v>
       </c>
       <c r="Y69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
       <c r="Z69">
@@ -4435,11 +5136,23 @@
       </c>
       <c r="F70" s="21"/>
       <c r="G70" s="20"/>
-      <c r="H70" s="14"/>
+      <c r="H70" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I70" s="15"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="14"/>
+      <c r="J70" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K70" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L70" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M70" s="22"/>
       <c r="N70" s="15"/>
       <c r="O70" s="2"/>
@@ -4462,7 +5175,7 @@
         <v>30</v>
       </c>
       <c r="Y70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>107</v>
       </c>
       <c r="Z70">
@@ -4483,11 +5196,23 @@
       </c>
       <c r="F71" s="21"/>
       <c r="G71" s="20"/>
-      <c r="H71" s="14"/>
+      <c r="H71" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I71" s="15"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="14"/>
+      <c r="J71" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K71" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L71" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M71" s="22"/>
       <c r="N71" s="15"/>
       <c r="O71" s="2"/>
@@ -4510,7 +5235,7 @@
         <v>30</v>
       </c>
       <c r="Y71">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="Z71">
@@ -4531,11 +5256,23 @@
       </c>
       <c r="F72" s="21"/>
       <c r="G72" s="20"/>
-      <c r="H72" s="14"/>
+      <c r="H72" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I72" s="15"/>
-      <c r="J72" s="5"/>
-      <c r="K72" s="5"/>
-      <c r="L72" s="14"/>
+      <c r="J72" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K72" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L72" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M72" s="22"/>
       <c r="N72" s="15"/>
       <c r="O72" s="2"/>
@@ -4558,7 +5295,7 @@
         <v>30</v>
       </c>
       <c r="Y72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>107</v>
       </c>
       <c r="Z72">
@@ -4579,11 +5316,23 @@
       </c>
       <c r="F73" s="21"/>
       <c r="G73" s="20"/>
-      <c r="H73" s="14"/>
+      <c r="H73" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I73" s="15"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="14"/>
+      <c r="J73" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K73" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L73" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M73" s="22"/>
       <c r="N73" s="15"/>
       <c r="O73" s="2"/>
@@ -4606,7 +5355,7 @@
         <v>30</v>
       </c>
       <c r="Y73">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>108</v>
       </c>
       <c r="Z73">
@@ -4627,11 +5376,23 @@
       </c>
       <c r="F74" s="21"/>
       <c r="G74" s="20"/>
-      <c r="H74" s="14"/>
+      <c r="H74" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I74" s="15"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="14"/>
+      <c r="J74" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K74" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L74" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="M74" s="22"/>
       <c r="N74" s="15"/>
       <c r="O74" s="2"/>
@@ -4654,7 +5415,7 @@
         <v>30</v>
       </c>
       <c r="Y74">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>109</v>
       </c>
       <c r="Z74">
@@ -4675,11 +5436,23 @@
       </c>
       <c r="F75" s="21"/>
       <c r="G75" s="20"/>
-      <c r="H75" s="14"/>
+      <c r="H75" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="I75" s="15"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="14"/>
+      <c r="J75" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K75" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L75" s="14">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
       <c r="M75" s="22"/>
       <c r="N75" s="15"/>
       <c r="O75" s="2"/>
@@ -4699,7 +5472,7 @@
         <v>19</v>
       </c>
       <c r="Y75">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
       <c r="Z75">
@@ -4720,11 +5493,23 @@
       </c>
       <c r="F76" s="21"/>
       <c r="G76" s="20"/>
-      <c r="H76" s="14"/>
+      <c r="H76" s="14">
+        <f t="shared" ref="H76:H92" si="5">IF((Y76)&gt;70,10,"")</f>
+        <v>10</v>
+      </c>
       <c r="I76" s="15"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="14"/>
+      <c r="J76" s="5">
+        <f t="shared" ref="J76:J92" si="6">IF((Y76)&gt;70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="K76" s="5">
+        <f t="shared" ref="K76:K92" si="7">IF((Y76)&gt;70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="L76" s="14">
+        <f t="shared" ref="L76:L93" si="8">IF((Y76)&gt;70,IF((Y76-50)&gt;50,50,IF((Y76-50)&lt;0,0,(Y76-50))), "" )</f>
+        <v>50</v>
+      </c>
       <c r="M76" s="22"/>
       <c r="N76" s="15"/>
       <c r="O76" s="2"/>
@@ -4747,7 +5532,7 @@
         <v>30</v>
       </c>
       <c r="Y76">
-        <f t="shared" ref="Y76:Y102" si="1">P76+(IF((Q76+R76+S76+T76)&gt;30,(Q76+R76+S76+T76)/4,IF((Q76+R76+S76+T76)&gt;20,(Q76+R76+S76+T76)/3,IF((Q76+R76+S76+T76)&gt;10,(Q76+R76+S76+T76)/2,(Q76+R76+S76+T76)))))+(U76*V76)+W76+X76+Z76</f>
+        <f t="shared" ref="Y76:Y102" si="9">P76+(IF((Q76+R76+S76+T76)&gt;30,(Q76+R76+S76+T76)/4,IF((Q76+R76+S76+T76)&gt;20,(Q76+R76+S76+T76)/3,IF((Q76+R76+S76+T76)&gt;10,(Q76+R76+S76+T76)/2,(Q76+R76+S76+T76)))))+(U76*V76)+W76+X76+Z76</f>
         <v>106</v>
       </c>
       <c r="Z76">
@@ -4768,11 +5553,23 @@
       </c>
       <c r="F77" s="21"/>
       <c r="G77" s="20"/>
-      <c r="H77" s="14"/>
+      <c r="H77" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I77" s="15"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="14"/>
+      <c r="J77" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K77" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L77" s="14">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
       <c r="M77" s="22"/>
       <c r="N77" s="15"/>
       <c r="O77" s="2"/>
@@ -4795,7 +5592,7 @@
         <v>30</v>
       </c>
       <c r="Y77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>108</v>
       </c>
       <c r="Z77">
@@ -4816,11 +5613,23 @@
       </c>
       <c r="F78" s="21"/>
       <c r="G78" s="20"/>
-      <c r="H78" s="14"/>
+      <c r="H78" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="I78" s="15"/>
-      <c r="J78" s="5"/>
-      <c r="K78" s="5"/>
-      <c r="L78" s="14"/>
+      <c r="J78" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="K78" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L78" s="14" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="M78" s="22"/>
       <c r="N78" s="15"/>
       <c r="O78" s="2"/>
@@ -4837,11 +5646,11 @@
         <v>30</v>
       </c>
       <c r="Y78">
-        <f t="shared" si="1"/>
-        <v>67</v>
+        <f t="shared" si="9"/>
+        <v>70</v>
       </c>
       <c r="Z78">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4858,11 +5667,23 @@
       </c>
       <c r="F79" s="21"/>
       <c r="G79" s="20"/>
-      <c r="H79" s="14"/>
+      <c r="H79" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I79" s="15"/>
-      <c r="J79" s="5"/>
-      <c r="K79" s="5"/>
-      <c r="L79" s="14"/>
+      <c r="J79" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K79" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L79" s="14">
+        <f t="shared" si="8"/>
+        <v>38</v>
+      </c>
       <c r="M79" s="22"/>
       <c r="N79" s="15"/>
       <c r="O79" s="2"/>
@@ -4885,7 +5706,7 @@
         <v>30</v>
       </c>
       <c r="Y79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>88</v>
       </c>
       <c r="Z79">
@@ -4906,11 +5727,23 @@
       </c>
       <c r="F80" s="21"/>
       <c r="G80" s="20"/>
-      <c r="H80" s="14"/>
+      <c r="H80" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I80" s="15"/>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-      <c r="L80" s="14"/>
+      <c r="J80" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K80" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L80" s="14">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
       <c r="M80" s="22"/>
       <c r="N80" s="15"/>
       <c r="O80" s="2"/>
@@ -4933,7 +5766,7 @@
         <v>30</v>
       </c>
       <c r="Y80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>111</v>
       </c>
       <c r="Z80">
@@ -4954,11 +5787,23 @@
       </c>
       <c r="F81" s="21"/>
       <c r="G81" s="20"/>
-      <c r="H81" s="14"/>
+      <c r="H81" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I81" s="15"/>
-      <c r="J81" s="5"/>
-      <c r="K81" s="5"/>
-      <c r="L81" s="14"/>
+      <c r="J81" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K81" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L81" s="14">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
       <c r="M81" s="22"/>
       <c r="N81" s="15"/>
       <c r="O81" s="2"/>
@@ -4981,7 +5826,7 @@
         <v>30</v>
       </c>
       <c r="Y81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="Z81">
@@ -5002,11 +5847,23 @@
       </c>
       <c r="F82" s="21"/>
       <c r="G82" s="20"/>
-      <c r="H82" s="14"/>
+      <c r="H82" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I82" s="15"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="5"/>
-      <c r="L82" s="14"/>
+      <c r="J82" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K82" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L82" s="14">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
       <c r="M82" s="22"/>
       <c r="N82" s="15"/>
       <c r="O82" s="2"/>
@@ -5029,7 +5886,7 @@
         <v>30</v>
       </c>
       <c r="Y82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>109</v>
       </c>
       <c r="Z82">
@@ -5050,11 +5907,23 @@
       </c>
       <c r="F83" s="21"/>
       <c r="G83" s="20"/>
-      <c r="H83" s="14"/>
+      <c r="H83" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I83" s="15"/>
-      <c r="J83" s="5"/>
-      <c r="K83" s="5"/>
-      <c r="L83" s="14"/>
+      <c r="J83" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K83" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L83" s="14">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
       <c r="M83" s="22"/>
       <c r="N83" s="15"/>
       <c r="O83" s="2"/>
@@ -5077,7 +5946,7 @@
         <v>30</v>
       </c>
       <c r="Y83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="Z83">
@@ -5098,11 +5967,23 @@
       </c>
       <c r="F84" s="21"/>
       <c r="G84" s="20"/>
-      <c r="H84" s="14"/>
+      <c r="H84" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I84" s="15"/>
-      <c r="J84" s="5"/>
-      <c r="K84" s="5"/>
-      <c r="L84" s="14"/>
+      <c r="J84" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K84" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L84" s="14">
+        <f t="shared" si="8"/>
+        <v>48</v>
+      </c>
       <c r="M84" s="22"/>
       <c r="N84" s="15"/>
       <c r="O84" s="2"/>
@@ -5125,7 +6006,7 @@
         <v>30</v>
       </c>
       <c r="Y84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>98</v>
       </c>
       <c r="Z84">
@@ -5146,11 +6027,23 @@
       </c>
       <c r="F85" s="21"/>
       <c r="G85" s="20"/>
-      <c r="H85" s="14"/>
+      <c r="H85" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I85" s="15"/>
-      <c r="J85" s="5"/>
-      <c r="K85" s="5"/>
-      <c r="L85" s="14"/>
+      <c r="J85" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K85" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L85" s="14">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
       <c r="M85" s="22"/>
       <c r="N85" s="15"/>
       <c r="O85" s="2"/>
@@ -5167,7 +6060,7 @@
         <v>30</v>
       </c>
       <c r="Y85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
       <c r="Z85">
@@ -5188,11 +6081,23 @@
       </c>
       <c r="F86" s="21"/>
       <c r="G86" s="20"/>
-      <c r="H86" s="14"/>
+      <c r="H86" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="I86" s="15"/>
-      <c r="J86" s="5"/>
-      <c r="K86" s="5"/>
-      <c r="L86" s="14"/>
+      <c r="J86" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="K86" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L86" s="14" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="M86" s="22"/>
       <c r="N86" s="15"/>
       <c r="O86" s="2"/>
@@ -5209,7 +6114,7 @@
         <v>30</v>
       </c>
       <c r="Y86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>56</v>
       </c>
       <c r="Z86">
@@ -5230,11 +6135,23 @@
       </c>
       <c r="F87" s="21"/>
       <c r="G87" s="20"/>
-      <c r="H87" s="14"/>
+      <c r="H87" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I87" s="15"/>
-      <c r="J87" s="5"/>
-      <c r="K87" s="5"/>
-      <c r="L87" s="14"/>
+      <c r="J87" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K87" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L87" s="14">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
       <c r="M87" s="22"/>
       <c r="N87" s="15"/>
       <c r="O87" s="2"/>
@@ -5257,7 +6174,7 @@
         <v>30</v>
       </c>
       <c r="Y87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>107</v>
       </c>
       <c r="Z87">
@@ -5278,11 +6195,23 @@
       </c>
       <c r="F88" s="21"/>
       <c r="G88" s="20"/>
-      <c r="H88" s="14"/>
+      <c r="H88" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="I88" s="15"/>
-      <c r="J88" s="5"/>
-      <c r="K88" s="5"/>
-      <c r="L88" s="14"/>
+      <c r="J88" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="K88" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L88" s="14" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="M88" s="22"/>
       <c r="N88" s="15"/>
       <c r="O88" s="2"/>
@@ -5296,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="Y88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>26</v>
       </c>
       <c r="Z88">
@@ -5317,11 +6246,23 @@
       </c>
       <c r="F89" s="21"/>
       <c r="G89" s="20"/>
-      <c r="H89" s="14"/>
+      <c r="H89" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I89" s="15"/>
-      <c r="J89" s="5"/>
-      <c r="K89" s="5"/>
-      <c r="L89" s="14"/>
+      <c r="J89" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K89" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L89" s="14">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
       <c r="M89" s="22"/>
       <c r="N89" s="15"/>
       <c r="O89" s="2"/>
@@ -5344,7 +6285,7 @@
         <v>-1</v>
       </c>
       <c r="Y89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>78</v>
       </c>
       <c r="Z89">
@@ -5365,11 +6306,23 @@
       </c>
       <c r="F90" s="21"/>
       <c r="G90" s="20"/>
-      <c r="H90" s="14"/>
+      <c r="H90" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I90" s="15"/>
-      <c r="J90" s="5"/>
-      <c r="K90" s="5"/>
-      <c r="L90" s="14"/>
+      <c r="J90" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K90" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L90" s="14">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
       <c r="M90" s="22"/>
       <c r="N90" s="15"/>
       <c r="O90" s="2"/>
@@ -5392,7 +6345,7 @@
         <v>30</v>
       </c>
       <c r="Y90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>106</v>
       </c>
       <c r="Z90">
@@ -5413,11 +6366,23 @@
       </c>
       <c r="F91" s="21"/>
       <c r="G91" s="20"/>
-      <c r="H91" s="14"/>
+      <c r="H91" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="I91" s="15"/>
-      <c r="J91" s="5"/>
-      <c r="K91" s="5"/>
-      <c r="L91" s="14"/>
+      <c r="J91" s="5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K91" s="5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="L91" s="14">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
       <c r="M91" s="22"/>
       <c r="N91" s="15"/>
       <c r="O91" s="2"/>
@@ -5434,7 +6399,7 @@
         <v>30</v>
       </c>
       <c r="Y91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>78</v>
       </c>
       <c r="Z91">
@@ -5455,11 +6420,23 @@
       </c>
       <c r="F92" s="21"/>
       <c r="G92" s="20"/>
-      <c r="H92" s="14"/>
+      <c r="H92" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="I92" s="15"/>
-      <c r="J92" s="5"/>
-      <c r="K92" s="5"/>
-      <c r="L92" s="14"/>
+      <c r="J92" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="K92" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L92" s="14" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="M92" s="22"/>
       <c r="N92" s="15"/>
       <c r="O92" s="2"/>
@@ -5476,11 +6453,11 @@
         <v>14</v>
       </c>
       <c r="Y92">
-        <f t="shared" si="1"/>
-        <v>56</v>
+        <f t="shared" si="9"/>
+        <v>70</v>
       </c>
       <c r="Z92">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:26" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5495,7 +6472,10 @@
       <c r="I93" s="15"/>
       <c r="J93" s="5"/>
       <c r="K93" s="5"/>
-      <c r="L93" s="14"/>
+      <c r="L93" s="14" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="M93" s="22"/>
       <c r="N93" s="15"/>
       <c r="O93" s="2"/>
@@ -5503,7 +6483,7 @@
         <v>1</v>
       </c>
       <c r="Y93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z93">
@@ -5530,7 +6510,7 @@
         <v>1</v>
       </c>
       <c r="Y94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z94">
@@ -5557,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="Y95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z95">
@@ -5584,7 +6564,7 @@
         <v>1</v>
       </c>
       <c r="Y96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z96">
@@ -5611,7 +6591,7 @@
         <v>1</v>
       </c>
       <c r="Y97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z97">
@@ -5638,7 +6618,7 @@
         <v>1</v>
       </c>
       <c r="Y98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z98">
@@ -5665,7 +6645,7 @@
         <v>1</v>
       </c>
       <c r="Y99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z99">
@@ -5692,7 +6672,7 @@
         <v>1</v>
       </c>
       <c r="Y100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z100">
@@ -5719,7 +6699,7 @@
         <v>1</v>
       </c>
       <c r="Y101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z101">
@@ -5746,7 +6726,7 @@
         <v>1</v>
       </c>
       <c r="Y102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Z102">

</xml_diff>